<commit_message>
final calculation is added
</commit_message>
<xml_diff>
--- a/Day14/Book1.xlsx
+++ b/Day14/Book1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d035d5460663dc91/Desktop/Selenium/Tutorial/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d035d5460663dc91/Desktop/Selenium/Tutorial/Day14/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5714BC63-86B5-4EBB-BDA9-D0C97F37502C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{494E9242-5A8D-41E3-8F3E-DB258B281D4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="10320" xr2:uid="{1F608D87-B770-488D-80CB-1AFE111933EE}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="10320" xr2:uid="{BF85BE80-4FAE-41EF-9B61-C22ED9AA4015}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,39 +33,36 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="11">
-  <si>
-    <t>BookName</t>
-  </si>
-  <si>
-    <t>Selenium</t>
-  </si>
-  <si>
-    <t>Java</t>
-  </si>
-  <si>
-    <t>Python</t>
-  </si>
-  <si>
-    <t>Jmeter</t>
-  </si>
-  <si>
-    <t>C#</t>
-  </si>
-  <si>
-    <t>PurchasedDate</t>
-  </si>
-  <si>
-    <t>Amount</t>
-  </si>
-  <si>
-    <t>Location</t>
-  </si>
-  <si>
-    <t>Africa</t>
-  </si>
-  <si>
-    <t>Asia</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="10">
+  <si>
+    <t>Principle</t>
+  </si>
+  <si>
+    <t>Rate of Interest</t>
+  </si>
+  <si>
+    <t>Period</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Maturity Value</t>
+  </si>
+  <si>
+    <t>Expected</t>
+  </si>
+  <si>
+    <t>Results</t>
+  </si>
+  <si>
+    <t>Simple Interest</t>
+  </si>
+  <si>
+    <t>Pass</t>
+  </si>
+  <si>
+    <t>Fail</t>
   </si>
 </sst>
 </file>
@@ -81,7 +78,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -91,6 +88,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -122,11 +131,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="15" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -440,102 +450,159 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E8699FC-F21B-46C8-BF82-86B705EF1DD3}">
-  <dimension ref="A1:D6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F983A9F2-58BC-4679-BC5A-9EA0FBA04BC4}">
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.85546875" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" customWidth="1"/>
+    <col min="7" max="7" width="12.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="3" t="s">
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>20000</v>
+      </c>
+      <c r="B2" s="1">
+        <v>10</v>
+      </c>
+      <c r="C2" s="1">
+        <v>2</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E2" s="1">
+        <v>24000</v>
+      </c>
+      <c r="F2" s="3" t="s">
         <v>8</v>
       </c>
+      <c r="G2" s="1"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="2">
-        <v>43675</v>
-      </c>
-      <c r="C2" s="1">
-        <v>350</v>
-      </c>
-      <c r="D2" s="1" t="s">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>40000</v>
+      </c>
+      <c r="B3" s="1">
+        <v>15</v>
+      </c>
+      <c r="C3" s="1">
+        <v>2</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="1">
+        <v>70000</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G3" s="1"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>50000</v>
+      </c>
+      <c r="B4" s="1">
+        <v>10</v>
+      </c>
+      <c r="C4" s="1">
+        <v>2</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="1">
+        <v>51250</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G4" s="1"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>75000</v>
+      </c>
+      <c r="B5" s="1">
+        <v>12</v>
+      </c>
+      <c r="C5" s="1">
+        <v>2</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="1">
+        <v>76500</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G5" s="1"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>75000</v>
+      </c>
+      <c r="B6" s="1">
+        <v>12</v>
+      </c>
+      <c r="C6" s="1">
+        <v>2</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="1">
+        <v>77043.320000000007</v>
+      </c>
+      <c r="F6" s="4" t="s">
         <v>9</v>
       </c>
+      <c r="G6" s="1"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="2">
-        <v>43675</v>
-      </c>
-      <c r="C3" s="1">
-        <v>200</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="2">
-        <v>43675</v>
-      </c>
-      <c r="C4" s="1">
-        <v>250</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="2">
-        <v>43675</v>
-      </c>
-      <c r="C5" s="1">
-        <v>150</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="2">
-        <v>43675</v>
-      </c>
-      <c r="C6" s="1">
-        <v>300</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>10</v>
-      </c>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>